<commit_message>
Added data import code, Added analysis, fixed a typo in simulator
</commit_message>
<xml_diff>
--- a/Bai_movObst2/schedule.xlsx
+++ b/Bai_movObst2/schedule.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5ABF21F-DBAB-4131-B030-6D4AA7CF6D08}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="21">
   <si>
     <t>subj_id</t>
   </si>
@@ -43,12 +44,51 @@
   </si>
   <si>
     <t>yes</t>
+  </si>
+  <si>
+    <t>Sumera</t>
+  </si>
+  <si>
+    <t>Megan</t>
+  </si>
+  <si>
+    <t>Tate</t>
+  </si>
+  <si>
+    <t>Christine</t>
+  </si>
+  <si>
+    <t>Mark</t>
+  </si>
+  <si>
+    <t>Natalie</t>
+  </si>
+  <si>
+    <t>Shruti</t>
+  </si>
+  <si>
+    <t>Cooro</t>
+  </si>
+  <si>
+    <t>Benita</t>
+  </si>
+  <si>
+    <t>Agusta</t>
+  </si>
+  <si>
+    <t>Ayush</t>
+  </si>
+  <si>
+    <t>Sue</t>
+  </si>
+  <si>
+    <t>Madeleine</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -359,16 +399,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+      <selection activeCell="R11" sqref="R11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="9.5703125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -382,7 +426,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -395,8 +439,14 @@
       <c r="D2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -409,8 +459,14 @@
       <c r="D3" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -423,8 +479,14 @@
       <c r="D4" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -437,8 +499,14 @@
       <c r="D5" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -451,8 +519,14 @@
       <c r="D6" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E6" t="s">
+        <v>12</v>
+      </c>
+      <c r="F6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -465,8 +539,14 @@
       <c r="D7" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -479,8 +559,14 @@
       <c r="D8" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E8" t="s">
+        <v>14</v>
+      </c>
+      <c r="F8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -493,8 +579,14 @@
       <c r="D9" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E9" t="s">
+        <v>15</v>
+      </c>
+      <c r="F9" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -507,8 +599,14 @@
       <c r="D10" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E10" t="s">
+        <v>16</v>
+      </c>
+      <c r="F10" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -521,8 +619,14 @@
       <c r="D11" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E11" t="s">
+        <v>17</v>
+      </c>
+      <c r="F11" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -535,8 +639,14 @@
       <c r="D12" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E12" t="s">
+        <v>18</v>
+      </c>
+      <c r="F12" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -548,6 +658,32 @@
       </c>
       <c r="D13" t="s">
         <v>7</v>
+      </c>
+      <c r="E13" t="s">
+        <v>19</v>
+      </c>
+      <c r="F13" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C14" t="s">
+        <v>4</v>
+      </c>
+      <c r="D14" t="s">
+        <v>6</v>
+      </c>
+      <c r="E14" t="s">
+        <v>20</v>
+      </c>
+      <c r="F14" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>